<commit_message>
python appium many devices
</commit_message>
<xml_diff>
--- a/testFile/userCase.xlsx
+++ b/testFile/userCase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20880" windowHeight="9930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20880" windowHeight="9930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summation" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>